<commit_message>
Loading works but Menu broke somehow its links
Editing menu broke it links and color settings on the buttons
</commit_message>
<xml_diff>
--- a/DesignFiles/Excel/Buildings.xlsx
+++ b/DesignFiles/Excel/Buildings.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F347E-A754-4079-A27E-52E3366A48C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11925" tabRatio="777" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="11925" tabRatio="777" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MarketBuilding" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="318">
   <si>
     <t>ID</t>
   </si>
@@ -980,6 +981,9 @@
   </si>
   <si>
     <t>Goat Farm</t>
+  </si>
+  <si>
+    <t>Fort</t>
   </si>
 </sst>
 </file>
@@ -3025,7 +3029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -5915,8 +5919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6027,13 +6031,7 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4">
-        <v>-1</v>
-      </c>
-      <c r="E4">
-        <v>206</v>
+        <v>317</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -6047,13 +6045,13 @@
         <v>1004</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="D5">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>293</v>
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>206</v>
       </c>
       <c r="G5">
         <v>3</v>
@@ -6067,13 +6065,13 @@
         <v>1005</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <v>21</v>
       </c>
-      <c r="E6">
-        <v>200</v>
+      <c r="E6" t="s">
+        <v>293</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -6087,13 +6085,13 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>296</v>
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>21</v>
       </c>
       <c r="E7">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -6107,19 +6105,33 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E8" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="E8">
+        <v>203</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
       <c r="H8">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E9" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>